<commit_message>
fixes to the drops
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200709_AW_special.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200709_AW_special.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="292">
   <si>
     <t>AGA Marks</t>
   </si>
@@ -1286,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AC156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView tabSelected="1" topLeftCell="Q6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q56" sqref="A56:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4788,9 +4788,6 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
-      <c r="AC53" s="2" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
@@ -4868,7 +4865,7 @@
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
       <c r="AC54" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.45">
@@ -4946,7 +4943,9 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
       <c r="AB55" s="1"/>
-      <c r="AC55" s="2"/>
+      <c r="AC55" s="2" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
@@ -5102,7 +5101,9 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
+      <c r="AC57" s="2" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
@@ -7023,7 +7024,6 @@
       <c r="Z82" s="1"/>
       <c r="AA82" s="1"/>
       <c r="AB82" s="1"/>
-      <c r="AC82" s="1"/>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
@@ -7101,7 +7101,7 @@
       <c r="AA83" s="1"/>
       <c r="AB83" s="1"/>
       <c r="AC83" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.45">
@@ -7180,7 +7180,7 @@
       <c r="AA84" s="1"/>
       <c r="AB84" s="1"/>
       <c r="AC84" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.45">
@@ -12360,7 +12360,6 @@
       <c r="Z151" s="1"/>
       <c r="AA151" s="1"/>
       <c r="AB151" s="1"/>
-      <c r="AC151" s="1"/>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A152" s="1" t="s">
@@ -12438,7 +12437,7 @@
       <c r="AA152" s="1"/>
       <c r="AB152" s="1"/>
       <c r="AC152" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.45">
@@ -12517,7 +12516,7 @@
       <c r="AA153" s="1"/>
       <c r="AB153" s="1"/>
       <c r="AC153" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.45">

</xml_diff>